<commit_message>
Update Olympic's fixtures list
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\Working stuffs\Analysis\Olympic FC\Data app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22358BAF-54CC-4667-ACDC-430982477177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E104504B-DD32-4BA7-A15D-DBEC22151111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,8 +464,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,8 +750,8 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>9</v>
+      <c r="G12" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -773,8 +773,8 @@
       <c r="F13" s="4">
         <v>2</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>9</v>
+      <c r="G13" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -842,8 +842,8 @@
       <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>9</v>
+      <c r="G16" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,8 +865,8 @@
       <c r="F17" s="4">
         <v>2</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
+      <c r="G17" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,8 +888,8 @@
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>9</v>
+      <c r="G18" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -911,8 +911,8 @@
       <c r="F19" s="4">
         <v>2</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>9</v>
+      <c r="G19" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,8 +934,8 @@
       <c r="F20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>9</v>
+      <c r="G20" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
       <c r="F21" s="4">
         <v>2</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update NPLQ data up to round 20
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E104504B-DD32-4BA7-A15D-DBEC22151111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F74C9E4-A2CA-4006-99A3-2DF333EAE4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,8 +464,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update NPLQ data up to round 21
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F74C9E4-A2CA-4006-99A3-2DF333EAE4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D96FE26-CCD4-47B9-9BEA-6F4E627559B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,8 +980,8 @@
       <c r="F22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>9</v>
+      <c r="G22" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update data and fixtures lists
Update include the data for NPLQ matches of round 22 and the catch-up matches, and changes made to the fixtures lists to include the Finals series (Semi-finals and Grand Final)
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D96FE26-CCD4-47B9-9BEA-6F4E627559B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF946CA-284D-4583-860A-67111A79767A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
   <si>
     <t>Round</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Sunshine Coast Wanderers</t>
+  </si>
+  <si>
+    <t>SF</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -155,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -462,10 +468,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1009,30 @@
       <c r="F23" s="4">
         <v>2</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>9</v>
+      </c>
+      <c r="F24" s="8">
+        <v>2</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update fixtures list to include the SF and GF
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF946CA-284D-4583-860A-67111A79767A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E18EA9A-3C75-425F-BDF1-782136F63A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
   <si>
     <t>Round</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>SF</t>
+  </si>
+  <si>
+    <t>GF</t>
   </si>
 </sst>
 </file>
@@ -143,20 +146,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -468,30 +466,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -500,7 +498,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -508,531 +506,554 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
         <v>27</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
         <v>27</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
         <v>17</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>4</v>
       </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
         <v>19</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
         <v>9</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>4</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
         <v>23</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>4</v>
       </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
         <v>5</v>
       </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3">
         <v>7</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>5</v>
       </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
         <v>4</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>6</v>
       </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
         <v>17</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>7</v>
       </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
         <v>13</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
-        <v>2</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3">
         <v>6</v>
       </c>
-      <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
         <v>18</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>6</v>
       </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
         <v>25</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>6</v>
       </c>
-      <c r="F16" s="4">
-        <v>2</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3">
         <v>3</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>7</v>
       </c>
-      <c r="F17" s="4">
-        <v>2</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3">
         <v>10</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>7</v>
       </c>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3">
         <v>23</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>7</v>
       </c>
-      <c r="F19" s="4">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="3">
         <v>30</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>7</v>
       </c>
-      <c r="F20" s="4">
-        <v>2</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3">
         <v>7</v>
       </c>
-      <c r="E21" s="4">
-        <v>8</v>
-      </c>
-      <c r="F21" s="4">
-        <v>2</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="E21" s="3">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="4">
-        <v>14</v>
-      </c>
-      <c r="E22" s="4">
-        <v>8</v>
-      </c>
-      <c r="F22" s="4">
-        <v>2</v>
-      </c>
-      <c r="G22" s="7" t="s">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="3">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3">
         <v>20</v>
       </c>
-      <c r="E23" s="4">
-        <v>8</v>
-      </c>
-      <c r="F23" s="4">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="E23" s="3">
+        <v>8</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="5">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1">
         <v>3</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="1">
         <v>9</v>
       </c>
-      <c r="F24" s="8">
-        <v>2</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploy app for the 2023 season
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EEE1A3-3F2C-43FD-B35E-0F3E4EB352BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D4A4EC-51F6-4A73-A95E-98E50E7FBC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
   <si>
     <t>Round</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Moreton Bay United</t>
   </si>
   <si>
-    <t>Logan Lightning</t>
-  </si>
-  <si>
-    <t>Capalaba</t>
-  </si>
-  <si>
     <t>Peninsula Power</t>
   </si>
   <si>
@@ -88,10 +82,10 @@
     <t>Sunshine Coast Wanderers</t>
   </si>
   <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>GF</t>
+    <t>Redlands United</t>
+  </si>
+  <si>
+    <t>Rochedale Rovers</t>
   </si>
 </sst>
 </file>
@@ -465,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,16 +501,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -530,13 +524,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3">
         <v>3</v>
@@ -553,16 +547,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -579,10 +573,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
@@ -599,16 +593,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -625,7 +619,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <v>9</v>
@@ -668,22 +662,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -691,13 +685,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
@@ -706,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,22 +708,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -737,22 +731,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -760,22 +754,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -783,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -798,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -806,10 +800,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
         <v>18</v>
@@ -821,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -832,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3">
         <v>25</v>
@@ -844,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,13 +846,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D17" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3">
         <v>7</v>
@@ -867,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -881,7 +875,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E18" s="3">
         <v>7</v>
@@ -890,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -913,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -921,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -936,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -944,13 +938,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3">
         <v>8</v>
@@ -959,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,14 +961,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="3">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3">
-        <v>14</v>
-      </c>
       <c r="E22" s="3">
         <v>8</v>
       </c>
@@ -982,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -990,13 +984,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="3">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E23" s="3">
         <v>8</v>
@@ -1005,54 +999,14 @@
         <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3</v>
-      </c>
-      <c r="E24" s="1">
-        <v>9</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1">
-        <v>9</v>
-      </c>
-      <c r="F25" s="4">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="F25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added data for Round 8
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\olympicdataapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D4A4EC-51F6-4A73-A95E-98E50E7FBC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DE39AC-2E22-48A5-B02E-FC5B915ACEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>